<commit_message>
Automatically was included 'estado' column to excel file, on response Email, 'enviado' o 'no_enviado'
</commit_message>
<xml_diff>
--- a/docs/cronograma1.xlsx
+++ b/docs/cronograma1.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esleyder\Desktop\email_sender\mailgun\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esleyder\Desktop\mailgun\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF60CAD-7420-4802-936D-95676F780D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C9CC01-EAEB-407E-8AAC-FD4ABD6100AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="15375" windowHeight="7995" xr2:uid="{509D5878-C751-42D2-8736-ABA362C8F363}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Eventos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>fecha</t>
   </si>
@@ -39,20 +34,29 @@
     <t>motivo</t>
   </si>
   <si>
+    <t>estado</t>
+  </si>
+  <si>
     <t>esleyder ordoñez</t>
   </si>
   <si>
+    <t>megaesleyder1@gmail.com</t>
+  </si>
+  <si>
     <t>Buenas tardes, recuerde que debe asistir a la actividad &lt;ACTIVIDAD&gt; en el lugar &lt;LUGAR&gt;, gracias por su atención</t>
   </si>
   <si>
-    <t>megaesleyder1@gmail.com</t>
+    <t>enviado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,20 +65,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -93,23 +86,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -122,7 +129,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -132,44 +139,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -196,32 +203,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -248,24 +237,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -277,196 +248,217 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0EC4058-978B-49C0-83F9-795254A10D27}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="102.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44966</v>
+        <v>44971</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D3" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{4A4F44B8-2653-402C-A12A-4B5E1CC13CFE}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
state in scheduler file
</commit_message>
<xml_diff>
--- a/docs/cronograma1.xlsx
+++ b/docs/cronograma1.xlsx
@@ -1,84 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esleyder\Desktop\mailgun\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C9CC01-EAEB-407E-8AAC-FD4ABD6100AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Eventos" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Eventos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>correo</t>
-  </si>
-  <si>
-    <t>motivo</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>esleyder ordoñez</t>
-  </si>
-  <si>
-    <t>megaesleyder1@gmail.com</t>
-  </si>
-  <si>
-    <t>Buenas tardes, recuerde que debe asistir a la actividad &lt;ACTIVIDAD&gt; en el lugar &lt;LUGAR&gt;, gracias por su atención</t>
-  </si>
-  <si>
-    <t>enviado</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -101,30 +68,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -412,50 +448,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>fecha</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>correo</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>motivo</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>estado</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2">
+      <c r="A2" s="4" t="n">
         <v>44971</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>esleyder ordoñez</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>megaesleyder1@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Buenas tardes, recuerde que debe asistir a la actividad &lt;ACTIVIDAD&gt; en el lugar &lt;LUGAR&gt;, gracias por su atención</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>enviado</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>